<commit_message>
Asset list update & keyspawn af
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List FPS.xlsx
+++ b/Algemeen/Asset List FPS.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="204">
   <si>
     <t>ID Code</t>
   </si>
@@ -620,6 +620,15 @@
   </si>
   <si>
     <t>H_KS_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intercom | Puzzles | </t>
+  </si>
+  <si>
+    <t>H_Int_01</t>
+  </si>
+  <si>
+    <t>H_P_01</t>
   </si>
 </sst>
 </file>
@@ -1093,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A347" sqref="A347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1623,11 +1632,9 @@
       </c>
       <c r="D19"/>
       <c r="E19"/>
-      <c r="H19" s="3" t="s">
-        <v>172</v>
-      </c>
+      <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1651,9 +1658,11 @@
       </c>
       <c r="D20"/>
       <c r="E20"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="I20" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1677,9 +1686,13 @@
       </c>
       <c r="D21"/>
       <c r="E21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
@@ -6081,34 +6094,34 @@
       <c r="E344"/>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A345" t="s">
-        <v>152</v>
-      </c>
-      <c r="B345" s="12" t="s">
-        <v>12</v>
+      <c r="A345" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B345" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C345" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="D345"/>
       <c r="E345"/>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A346" t="s">
-        <v>153</v>
-      </c>
-      <c r="B346" s="12" t="s">
-        <v>12</v>
+      <c r="A346" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B346" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C346" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="D346"/>
       <c r="E346"/>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B347" s="12" t="s">
         <v>12</v>
@@ -6121,7 +6134,7 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B348" s="12" t="s">
         <v>12</v>
@@ -6134,7 +6147,7 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B349" s="12" t="s">
         <v>12</v>
@@ -6147,7 +6160,7 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B350" s="12" t="s">
         <v>12</v>
@@ -6160,7 +6173,7 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B351" s="12" t="s">
         <v>12</v>
@@ -6173,7 +6186,7 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B352" s="12" t="s">
         <v>12</v>
@@ -6186,7 +6199,7 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B353" s="12" t="s">
         <v>12</v>
@@ -6199,7 +6212,7 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B354" s="12" t="s">
         <v>12</v>
@@ -6212,7 +6225,7 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B355" s="12" t="s">
         <v>12</v>
@@ -6225,7 +6238,7 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B356" s="12" t="s">
         <v>12</v>
@@ -6238,7 +6251,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B357" s="12" t="s">
         <v>12</v>
@@ -6251,7 +6264,7 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B358" s="12" t="s">
         <v>12</v>
@@ -6264,7 +6277,7 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B359" s="12" t="s">
         <v>12</v>
@@ -6277,7 +6290,7 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B360" s="12" t="s">
         <v>12</v>
@@ -6290,7 +6303,7 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B361" s="12" t="s">
         <v>12</v>
@@ -6303,7 +6316,7 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B362" s="12" t="s">
         <v>12</v>
@@ -6315,16 +6328,28 @@
       <c r="E362"/>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A363"/>
-      <c r="B363"/>
-      <c r="C363"/>
+      <c r="A363" t="s">
+        <v>168</v>
+      </c>
+      <c r="B363" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C363" t="s">
+        <v>170</v>
+      </c>
       <c r="D363"/>
       <c r="E363"/>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A364"/>
-      <c r="B364"/>
-      <c r="C364"/>
+      <c r="A364" t="s">
+        <v>169</v>
+      </c>
+      <c r="B364" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C364" t="s">
+        <v>170</v>
+      </c>
       <c r="D364"/>
       <c r="E364"/>
     </row>

</xml_diff>

<commit_message>
asset list changes & update.
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List FPS.xlsx
+++ b/Algemeen/Asset List FPS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="207">
   <si>
     <t>ID Code</t>
   </si>
@@ -622,9 +622,6 @@
     <t>H_KS_01</t>
   </si>
   <si>
-    <t xml:space="preserve">Intercom | Puzzles | </t>
-  </si>
-  <si>
     <t>H_Int_01</t>
   </si>
   <si>
@@ -635,6 +632,12 @@
   </si>
   <si>
     <t>H_EMo_01</t>
+  </si>
+  <si>
+    <t>H_MCo_01</t>
+  </si>
+  <si>
+    <t>Intercom | Puzzles | MeleeCombat |</t>
   </si>
 </sst>
 </file>
@@ -1112,32 +1115,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F283" sqref="F283"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="33" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1193,7 +1196,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1220,7 +1223,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1253,7 +1256,7 @@
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1286,7 +1289,7 @@
       <c r="Q5"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1319,7 +1322,7 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1352,7 +1355,7 @@
       <c r="Q7"/>
       <c r="R7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1383,7 +1386,7 @@
       <c r="Q8"/>
       <c r="R8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1414,7 +1417,7 @@
       <c r="Q9"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1445,7 +1448,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1473,7 +1476,7 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1501,7 +1504,7 @@
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1529,7 +1532,7 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1559,7 +1562,7 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1587,7 +1590,7 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1617,7 +1620,7 @@
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1645,7 +1648,7 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1673,7 +1676,7 @@
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1689,7 +1692,7 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1701,7 +1704,7 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1731,7 +1734,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1759,7 +1762,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1783,7 +1786,7 @@
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1807,7 +1810,7 @@
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1831,7 +1834,7 @@
       <c r="Q24"/>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1855,7 +1858,7 @@
       <c r="Q25"/>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1879,7 +1882,7 @@
       <c r="Q26"/>
       <c r="R26"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1903,7 +1906,7 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1927,7 +1930,7 @@
       <c r="Q28"/>
       <c r="R28"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1951,7 +1954,7 @@
       <c r="Q29"/>
       <c r="R29"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1975,7 +1978,7 @@
       <c r="Q30"/>
       <c r="R30"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2000,7 +2003,7 @@
       <c r="Q31"/>
       <c r="R31"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2026,7 +2029,7 @@
       <c r="Q32"/>
       <c r="R32"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>57</v>
       </c>
@@ -2052,7 +2055,7 @@
       <c r="Q33"/>
       <c r="R33"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>57</v>
       </c>
@@ -2078,7 +2081,7 @@
       <c r="Q34"/>
       <c r="R34"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>57</v>
       </c>
@@ -2104,7 +2107,7 @@
       <c r="Q35"/>
       <c r="R35"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>57</v>
       </c>
@@ -2130,7 +2133,7 @@
       <c r="Q36"/>
       <c r="R36"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>57</v>
       </c>
@@ -2156,7 +2159,7 @@
       <c r="Q37"/>
       <c r="R37"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>57</v>
       </c>
@@ -2173,7 +2176,7 @@
       <c r="I38" s="16"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -2190,7 +2193,7 @@
       <c r="I39" s="16"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -2207,7 +2210,7 @@
       <c r="I40" s="2"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>59</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>59</v>
       </c>
@@ -2252,7 +2255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>59</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>59</v>
       </c>
@@ -2282,7 +2285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>59</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>55</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>55</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
         <v>55</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>55</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>55</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>55</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
         <v>56</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
         <v>56</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
         <v>56</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
         <v>56</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
         <v>56</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>56</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>60</v>
       </c>
@@ -2582,7 +2585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>60</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
         <v>60</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
         <v>60</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>60</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
         <v>60</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -2672,7 +2675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -2747,7 +2750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>63</v>
       </c>
@@ -2762,7 +2765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>63</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>63</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>63</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>64</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>61</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>61</v>
       </c>
@@ -2852,7 +2855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>61</v>
       </c>
@@ -2867,7 +2870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>61</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
         <v>61</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>61</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>61</v>
       </c>
@@ -2927,7 +2930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>61</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>62</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>65</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>123</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
         <v>123</v>
       </c>
@@ -3002,7 +3005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="19" t="s">
         <v>123</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
         <v>123</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>123</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>123</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="19" t="s">
         <v>89</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="19" t="s">
         <v>89</v>
       </c>
@@ -3092,7 +3095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="19" t="s">
         <v>89</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="19" t="s">
         <v>119</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
         <v>119</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="19" t="s">
         <v>119</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
         <v>131</v>
       </c>
@@ -3167,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
         <v>131</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="19" t="s">
         <v>131</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -3212,7 +3215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>122</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>115</v>
       </c>
@@ -3257,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -3272,7 +3275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -3287,7 +3290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>96</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>96</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>96</v>
       </c>
@@ -3332,7 +3335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="19" t="s">
         <v>127</v>
       </c>
@@ -3347,7 +3350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="19" t="s">
         <v>127</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="19" t="s">
         <v>127</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>121</v>
       </c>
@@ -3392,7 +3395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -3422,7 +3425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>67</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>67</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>67</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>86</v>
       </c>
@@ -3482,7 +3485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>86</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>86</v>
       </c>
@@ -3512,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -3527,7 +3530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>118</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>118</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="19" t="s">
         <v>74</v>
       </c>
@@ -3573,7 +3576,7 @@
       </c>
       <c r="F131"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="19" t="s">
         <v>74</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="19" t="s">
         <v>74</v>
       </c>
@@ -3604,7 +3607,7 @@
       </c>
       <c r="G133" s="14"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="19" t="s">
         <v>74</v>
       </c>
@@ -3621,7 +3624,7 @@
       <c r="F134"/>
       <c r="G134" s="14"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>74</v>
       </c>
@@ -3638,7 +3641,7 @@
       <c r="F135"/>
       <c r="G135" s="14"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>74</v>
       </c>
@@ -3654,7 +3657,7 @@
       </c>
       <c r="G136" s="14"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>110</v>
       </c>
@@ -3670,7 +3673,7 @@
       </c>
       <c r="G137" s="14"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>110</v>
       </c>
@@ -3686,7 +3689,7 @@
       </c>
       <c r="G138" s="14"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>110</v>
       </c>
@@ -3702,7 +3705,7 @@
       </c>
       <c r="G139" s="14"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>113</v>
       </c>
@@ -3718,7 +3721,7 @@
       </c>
       <c r="G140" s="14"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>113</v>
       </c>
@@ -3734,7 +3737,7 @@
       </c>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>113</v>
       </c>
@@ -3750,7 +3753,7 @@
       </c>
       <c r="G142" s="14"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="19" t="s">
         <v>102</v>
       </c>
@@ -3766,7 +3769,7 @@
       </c>
       <c r="G143" s="14"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="19" t="s">
         <v>102</v>
       </c>
@@ -3782,7 +3785,7 @@
       </c>
       <c r="G144" s="14"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="19" t="s">
         <v>102</v>
       </c>
@@ -3798,7 +3801,7 @@
       </c>
       <c r="G145" s="14"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>103</v>
       </c>
@@ -3814,7 +3817,7 @@
       </c>
       <c r="G146" s="14"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>103</v>
       </c>
@@ -3830,7 +3833,7 @@
       </c>
       <c r="G147" s="14"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>103</v>
       </c>
@@ -3846,7 +3849,7 @@
       </c>
       <c r="G148" s="14"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>103</v>
       </c>
@@ -3862,7 +3865,7 @@
       </c>
       <c r="G149" s="14"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>103</v>
       </c>
@@ -3878,7 +3881,7 @@
       </c>
       <c r="G150" s="14"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>71</v>
       </c>
@@ -3894,7 +3897,7 @@
       </c>
       <c r="G151" s="14"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>71</v>
       </c>
@@ -3910,7 +3913,7 @@
       </c>
       <c r="G152" s="14"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>71</v>
       </c>
@@ -3926,7 +3929,7 @@
       </c>
       <c r="G153" s="14"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>70</v>
       </c>
@@ -3942,7 +3945,7 @@
       </c>
       <c r="G154" s="14"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>70</v>
       </c>
@@ -3958,7 +3961,7 @@
       </c>
       <c r="G155" s="14"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>70</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>92</v>
       </c>
@@ -3988,7 +3991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>92</v>
       </c>
@@ -4003,7 +4006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>92</v>
       </c>
@@ -4018,7 +4021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>112</v>
       </c>
@@ -4033,7 +4036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>112</v>
       </c>
@@ -4048,7 +4051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>112</v>
       </c>
@@ -4063,7 +4066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="19" t="s">
         <v>130</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="19" t="s">
         <v>130</v>
       </c>
@@ -4093,7 +4096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="19" t="s">
         <v>130</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>78</v>
       </c>
@@ -4123,7 +4126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>78</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>78</v>
       </c>
@@ -4153,7 +4156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="19" t="s">
         <v>93</v>
       </c>
@@ -4168,7 +4171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="19" t="s">
         <v>93</v>
       </c>
@@ -4183,7 +4186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="19" t="s">
         <v>93</v>
       </c>
@@ -4198,7 +4201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="19" t="s">
         <v>94</v>
       </c>
@@ -4213,7 +4216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="19" t="s">
         <v>94</v>
       </c>
@@ -4228,7 +4231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="19" t="s">
         <v>94</v>
       </c>
@@ -4243,7 +4246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="19" t="s">
         <v>124</v>
       </c>
@@ -4258,7 +4261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="19" t="s">
         <v>124</v>
       </c>
@@ -4273,7 +4276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="19" t="s">
         <v>124</v>
       </c>
@@ -4288,7 +4291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>106</v>
       </c>
@@ -4303,7 +4306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>106</v>
       </c>
@@ -4318,7 +4321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>106</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="19" t="s">
         <v>116</v>
       </c>
@@ -4348,7 +4351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="19" t="s">
         <v>116</v>
       </c>
@@ -4363,7 +4366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="19" t="s">
         <v>116</v>
       </c>
@@ -4378,7 +4381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="19" t="s">
         <v>117</v>
       </c>
@@ -4393,7 +4396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="19" t="s">
         <v>117</v>
       </c>
@@ -4408,7 +4411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="19" t="s">
         <v>117</v>
       </c>
@@ -4423,7 +4426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>126</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>126</v>
       </c>
@@ -4454,7 +4457,7 @@
       </c>
       <c r="F188" s="2"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>126</v>
       </c>
@@ -4469,7 +4472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="19" t="s">
         <v>72</v>
       </c>
@@ -4484,7 +4487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="19" t="s">
         <v>72</v>
       </c>
@@ -4499,7 +4502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="19" t="s">
         <v>72</v>
       </c>
@@ -4514,7 +4517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>91</v>
       </c>
@@ -4529,7 +4532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>91</v>
       </c>
@@ -4544,7 +4547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>91</v>
       </c>
@@ -4559,7 +4562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>109</v>
       </c>
@@ -4574,7 +4577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>109</v>
       </c>
@@ -4589,7 +4592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>109</v>
       </c>
@@ -4604,7 +4607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>95</v>
       </c>
@@ -4619,7 +4622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>95</v>
       </c>
@@ -4634,7 +4637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>95</v>
       </c>
@@ -4649,9 +4652,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B202" s="7" t="s">
         <v>13</v>
@@ -4664,9 +4667,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B203" s="15" t="s">
         <v>10</v>
@@ -4679,9 +4682,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B204" s="8" t="s">
         <v>14</v>
@@ -4694,7 +4697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>107</v>
       </c>
@@ -4709,7 +4712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>107</v>
       </c>
@@ -4724,7 +4727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>107</v>
       </c>
@@ -4739,7 +4742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>82</v>
       </c>
@@ -4754,7 +4757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>82</v>
       </c>
@@ -4769,7 +4772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>82</v>
       </c>
@@ -4784,7 +4787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="19" t="s">
         <v>77</v>
       </c>
@@ -4799,7 +4802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="19" t="s">
         <v>77</v>
       </c>
@@ -4814,7 +4817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="19" t="s">
         <v>77</v>
       </c>
@@ -4829,7 +4832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>97</v>
       </c>
@@ -4844,7 +4847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>97</v>
       </c>
@@ -4859,7 +4862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>97</v>
       </c>
@@ -4874,7 +4877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>114</v>
       </c>
@@ -4889,7 +4892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>114</v>
       </c>
@@ -4904,7 +4907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>114</v>
       </c>
@@ -4919,7 +4922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>80</v>
       </c>
@@ -4934,7 +4937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>80</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>80</v>
       </c>
@@ -4964,7 +4967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>129</v>
       </c>
@@ -4979,7 +4982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>129</v>
       </c>
@@ -4994,7 +4997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>129</v>
       </c>
@@ -5009,7 +5012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>75</v>
       </c>
@@ -5024,7 +5027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>75</v>
       </c>
@@ -5039,7 +5042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>75</v>
       </c>
@@ -5054,7 +5057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="19" t="s">
         <v>76</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="19" t="s">
         <v>76</v>
       </c>
@@ -5084,7 +5087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="19" t="s">
         <v>76</v>
       </c>
@@ -5099,7 +5102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>79</v>
       </c>
@@ -5114,7 +5117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>79</v>
       </c>
@@ -5129,7 +5132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>79</v>
       </c>
@@ -5144,7 +5147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>99</v>
       </c>
@@ -5159,7 +5162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>99</v>
       </c>
@@ -5174,7 +5177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>99</v>
       </c>
@@ -5189,7 +5192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>83</v>
       </c>
@@ -5204,7 +5207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>83</v>
       </c>
@@ -5219,7 +5222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>83</v>
       </c>
@@ -5234,7 +5237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>84</v>
       </c>
@@ -5249,7 +5252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>84</v>
       </c>
@@ -5264,7 +5267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>84</v>
       </c>
@@ -5279,7 +5282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>73</v>
       </c>
@@ -5294,7 +5297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>73</v>
       </c>
@@ -5309,7 +5312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>73</v>
       </c>
@@ -5324,7 +5327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="19" t="s">
         <v>81</v>
       </c>
@@ -5339,7 +5342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="19" t="s">
         <v>81</v>
       </c>
@@ -5354,7 +5357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="19" t="s">
         <v>81</v>
       </c>
@@ -5369,7 +5372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="19" t="s">
         <v>81</v>
       </c>
@@ -5384,7 +5387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>81</v>
       </c>
@@ -5399,7 +5402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>81</v>
       </c>
@@ -5414,7 +5417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>128</v>
       </c>
@@ -5429,7 +5432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>128</v>
       </c>
@@ -5444,7 +5447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>128</v>
       </c>
@@ -5459,7 +5462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>68</v>
       </c>
@@ -5474,7 +5477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>68</v>
       </c>
@@ -5489,7 +5492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>68</v>
       </c>
@@ -5504,7 +5507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>68</v>
       </c>
@@ -5519,7 +5522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>68</v>
       </c>
@@ -5534,7 +5537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>68</v>
       </c>
@@ -5549,7 +5552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>105</v>
       </c>
@@ -5564,7 +5567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>105</v>
       </c>
@@ -5579,7 +5582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>105</v>
       </c>
@@ -5594,7 +5597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>104</v>
       </c>
@@ -5609,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>104</v>
       </c>
@@ -5624,7 +5627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>104</v>
       </c>
@@ -5639,7 +5642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>69</v>
       </c>
@@ -5654,7 +5657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>69</v>
       </c>
@@ -5669,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>69</v>
       </c>
@@ -5684,7 +5687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>111</v>
       </c>
@@ -5699,7 +5702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>111</v>
       </c>
@@ -5714,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>111</v>
       </c>
@@ -5729,7 +5732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>88</v>
       </c>
@@ -5744,7 +5747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>88</v>
       </c>
@@ -5759,7 +5762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>88</v>
       </c>
@@ -5774,7 +5777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="19" t="s">
         <v>101</v>
       </c>
@@ -5789,7 +5792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="19" t="s">
         <v>101</v>
       </c>
@@ -5804,7 +5807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="19" t="s">
         <v>101</v>
       </c>
@@ -5819,7 +5822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="19" t="s">
         <v>125</v>
       </c>
@@ -5834,7 +5837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="19" t="s">
         <v>125</v>
       </c>
@@ -5849,7 +5852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="19" t="s">
         <v>125</v>
       </c>
@@ -5864,7 +5867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>90</v>
       </c>
@@ -5879,7 +5882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>90</v>
       </c>
@@ -5894,7 +5897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>90</v>
       </c>
@@ -5909,7 +5912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>108</v>
       </c>
@@ -5924,7 +5927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>108</v>
       </c>
@@ -5939,7 +5942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>108</v>
       </c>
@@ -5954,7 +5957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="19" t="s">
         <v>66</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="19" t="s">
         <v>66</v>
       </c>
@@ -5984,7 +5987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="19" t="s">
         <v>66</v>
       </c>
@@ -5999,7 +6002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>98</v>
       </c>
@@ -6014,7 +6017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>98</v>
       </c>
@@ -6029,7 +6032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>98</v>
       </c>
@@ -6044,7 +6047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>87</v>
       </c>
@@ -6059,7 +6062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>87</v>
       </c>
@@ -6074,7 +6077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>87</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>100</v>
       </c>
@@ -6104,7 +6107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>100</v>
       </c>
@@ -6119,7 +6122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>100</v>
       </c>
@@ -6134,7 +6137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>85</v>
       </c>
@@ -6149,7 +6152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>85</v>
       </c>
@@ -6164,7 +6167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>85</v>
       </c>
@@ -6179,7 +6182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>120</v>
       </c>
@@ -6194,7 +6197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>120</v>
       </c>
@@ -6209,7 +6212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>120</v>
       </c>
@@ -6224,7 +6227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>145</v>
       </c>
@@ -6239,7 +6242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -6254,7 +6257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>139</v>
       </c>
@@ -6269,7 +6272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>146</v>
       </c>
@@ -6284,7 +6287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>143</v>
       </c>
@@ -6299,7 +6302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>142</v>
       </c>
@@ -6314,7 +6317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>147</v>
       </c>
@@ -6329,7 +6332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>136</v>
       </c>
@@ -6344,7 +6347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>134</v>
       </c>
@@ -6359,7 +6362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>137</v>
       </c>
@@ -6374,7 +6377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>138</v>
       </c>
@@ -6389,7 +6392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>141</v>
       </c>
@@ -6404,7 +6407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>132</v>
       </c>
@@ -6419,7 +6422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>140</v>
       </c>
@@ -6434,7 +6437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>144</v>
       </c>
@@ -6449,7 +6452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>197</v>
       </c>
@@ -6464,7 +6467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>186</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>187</v>
       </c>
@@ -6494,7 +6497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>188</v>
       </c>
@@ -6509,7 +6512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>191</v>
       </c>
@@ -6524,7 +6527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>181</v>
       </c>
@@ -6539,7 +6542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="19" t="s">
         <v>196</v>
       </c>
@@ -6554,7 +6557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>198</v>
       </c>
@@ -6569,7 +6572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="19" t="s">
         <v>183</v>
       </c>
@@ -6584,9 +6587,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B331" s="11" t="s">
         <v>15</v>
@@ -6598,7 +6601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>182</v>
       </c>
@@ -6613,7 +6616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>148</v>
       </c>
@@ -6628,7 +6631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="19" t="s">
         <v>179</v>
       </c>
@@ -6643,7 +6646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="19" t="s">
         <v>180</v>
       </c>
@@ -6658,7 +6661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="19" t="s">
         <v>178</v>
       </c>
@@ -6673,7 +6676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>194</v>
       </c>
@@ -6688,9 +6691,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B338" s="11" t="s">
         <v>15</v>
@@ -6703,7 +6706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="19" t="s">
         <v>192</v>
       </c>
@@ -6718,7 +6721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>200</v>
       </c>
@@ -6733,7 +6736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="19" t="s">
         <v>193</v>
       </c>
@@ -6748,7 +6751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="19" t="s">
         <v>176</v>
       </c>
@@ -6763,7 +6766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="19" t="s">
         <v>175</v>
       </c>
@@ -6778,9 +6781,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B344" s="11" t="s">
         <v>15</v>
@@ -6793,7 +6796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="19" t="s">
         <v>177</v>
       </c>
@@ -6808,7 +6811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>190</v>
       </c>
@@ -6823,7 +6826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>184</v>
       </c>
@@ -6838,7 +6841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>189</v>
       </c>
@@ -6853,7 +6856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>195</v>
       </c>
@@ -6868,7 +6871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>185</v>
       </c>
@@ -6883,7 +6886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>169</v>
       </c>
@@ -6898,7 +6901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>156</v>
       </c>
@@ -6913,7 +6916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>160</v>
       </c>
@@ -6928,7 +6931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>154</v>
       </c>
@@ -6943,7 +6946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>155</v>
       </c>
@@ -6958,7 +6961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>162</v>
       </c>
@@ -6973,7 +6976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>152</v>
       </c>
@@ -6988,7 +6991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>158</v>
       </c>
@@ -7003,7 +7006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>157</v>
       </c>
@@ -7018,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>161</v>
       </c>
@@ -7033,7 +7036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>166</v>
       </c>
@@ -7048,7 +7051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>167</v>
       </c>
@@ -7063,7 +7066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>153</v>
       </c>
@@ -7078,7 +7081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>165</v>
       </c>
@@ -7093,7 +7096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>163</v>
       </c>
@@ -7108,7 +7111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>168</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>164</v>
       </c>
@@ -7138,7 +7141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>159</v>
       </c>
@@ -7153,639 +7156,653 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A369" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B369" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C369" t="s">
+        <v>149</v>
+      </c>
+      <c r="E369" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384"/>
       <c r="B384"/>
       <c r="C384"/>
       <c r="D384"/>
       <c r="E384"/>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385"/>
       <c r="B385"/>
       <c r="C385"/>
       <c r="D385"/>
       <c r="E385"/>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386"/>
       <c r="B386"/>
       <c r="C386"/>
       <c r="D386"/>
       <c r="E386"/>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387"/>
       <c r="B387"/>
       <c r="C387"/>
       <c r="D387"/>
       <c r="E387"/>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388"/>
       <c r="B388"/>
       <c r="C388"/>
       <c r="D388"/>
       <c r="E388"/>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389"/>
       <c r="B389"/>
       <c r="C389"/>
       <c r="D389"/>
       <c r="E389"/>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390"/>
       <c r="B390"/>
       <c r="C390"/>
       <c r="D390"/>
       <c r="E390"/>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391"/>
       <c r="B391"/>
       <c r="C391"/>
       <c r="D391"/>
       <c r="E391"/>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392"/>
       <c r="B392"/>
       <c r="C392"/>
       <c r="D392"/>
       <c r="E392"/>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393"/>
       <c r="B393"/>
       <c r="C393"/>
       <c r="D393"/>
       <c r="E393"/>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394"/>
       <c r="B394"/>
       <c r="C394"/>
       <c r="D394"/>
       <c r="E394"/>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395"/>
       <c r="B395"/>
       <c r="C395"/>
       <c r="D395"/>
       <c r="E395"/>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396"/>
       <c r="B396"/>
       <c r="C396"/>
       <c r="D396"/>
       <c r="E396"/>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D397"/>
       <c r="E397"/>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D398"/>
       <c r="E398"/>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D399"/>
       <c r="E399"/>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D400"/>
       <c r="E400"/>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D401"/>
       <c r="E401"/>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D402"/>
       <c r="E402"/>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D403"/>
       <c r="E403"/>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D404"/>
       <c r="E404"/>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D405"/>
       <c r="E405"/>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D406"/>
       <c r="E406"/>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D407"/>
       <c r="E407"/>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D408"/>
       <c r="E408"/>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D409"/>
       <c r="E409"/>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D410"/>
       <c r="E410"/>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D411"/>
       <c r="E411"/>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D412"/>
       <c r="E412"/>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D413"/>
       <c r="E413"/>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D414"/>
       <c r="E414"/>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415"/>
       <c r="B415"/>
       <c r="C415"/>
       <c r="D415"/>
       <c r="E415"/>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416"/>
       <c r="B416"/>
       <c r="C416"/>
       <c r="D416"/>
       <c r="E416"/>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417"/>
       <c r="B417"/>
       <c r="C417"/>
       <c r="D417"/>
       <c r="E417"/>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418"/>
       <c r="B418"/>
       <c r="C418"/>
       <c r="D418"/>
       <c r="E418"/>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419"/>
       <c r="B419"/>
       <c r="C419"/>
       <c r="D419"/>
       <c r="E419"/>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420"/>
       <c r="B420"/>
       <c r="C420"/>
       <c r="D420"/>
       <c r="E420"/>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421"/>
       <c r="B421"/>
       <c r="C421"/>
       <c r="D421"/>
       <c r="E421"/>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422"/>
       <c r="B422"/>
       <c r="C422"/>
       <c r="D422"/>
       <c r="E422"/>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423"/>
       <c r="B423"/>
       <c r="C423"/>
       <c r="D423"/>
       <c r="E423"/>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424"/>
       <c r="B424"/>
       <c r="C424"/>
       <c r="D424"/>
       <c r="E424"/>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425"/>
       <c r="B425"/>
       <c r="C425"/>
       <c r="D425"/>
       <c r="E425"/>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426"/>
       <c r="B426"/>
       <c r="C426"/>
       <c r="D426"/>
       <c r="E426"/>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427"/>
       <c r="B427"/>
       <c r="C427"/>
       <c r="D427"/>
       <c r="E427"/>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428"/>
       <c r="B428"/>
       <c r="C428"/>
       <c r="D428"/>
       <c r="E428"/>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429"/>
       <c r="B429"/>
       <c r="C429"/>
       <c r="D429"/>
       <c r="E429"/>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430"/>
       <c r="B430"/>
       <c r="C430"/>
       <c r="D430"/>
       <c r="E430"/>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431"/>
       <c r="B431"/>
       <c r="C431"/>
       <c r="D431"/>
       <c r="E431"/>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432"/>
       <c r="B432"/>
       <c r="C432"/>
       <c r="D432"/>
       <c r="E432"/>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433"/>
       <c r="B433"/>
       <c r="C433"/>
       <c r="D433"/>
       <c r="E433"/>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434"/>
       <c r="B434"/>
       <c r="C434"/>
       <c r="D434"/>
       <c r="E434"/>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435"/>
       <c r="B435"/>
       <c r="C435"/>
       <c r="D435"/>
       <c r="E435"/>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436"/>
       <c r="B436"/>
       <c r="C436"/>
       <c r="D436"/>
       <c r="E436"/>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437"/>
       <c r="B437"/>
       <c r="C437"/>
       <c r="D437"/>
       <c r="E437"/>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A438"/>
       <c r="B438"/>
       <c r="C438"/>
       <c r="D438"/>
       <c r="E438"/>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439"/>
       <c r="B439"/>
       <c r="C439"/>
       <c r="D439"/>
       <c r="E439"/>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440"/>
       <c r="B440"/>
       <c r="C440"/>
       <c r="D440"/>
       <c r="E440"/>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441"/>
       <c r="B441"/>
       <c r="C441"/>
       <c r="D441"/>
       <c r="E441"/>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442"/>
       <c r="B442"/>
       <c r="C442"/>
       <c r="D442"/>
       <c r="E442"/>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443"/>
       <c r="B443"/>
       <c r="C443"/>
       <c r="D443"/>
       <c r="E443"/>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444"/>
       <c r="B444"/>
       <c r="C444"/>
       <c r="D444"/>
       <c r="E444"/>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445"/>
       <c r="B445"/>
       <c r="C445"/>
       <c r="D445"/>
       <c r="E445"/>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446"/>
       <c r="B446"/>
       <c r="C446"/>
       <c r="D446"/>
       <c r="E446"/>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447"/>
       <c r="B447"/>
       <c r="C447"/>
       <c r="D447"/>
       <c r="E447"/>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A448"/>
       <c r="B448"/>
       <c r="C448"/>
       <c r="D448"/>
       <c r="E448"/>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A449"/>
       <c r="B449"/>
       <c r="C449"/>
       <c r="D449"/>
       <c r="E449"/>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450"/>
       <c r="B450"/>
       <c r="C450"/>
       <c r="D450"/>
       <c r="E450"/>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451"/>
       <c r="B451"/>
       <c r="C451"/>
       <c r="D451"/>
       <c r="E451"/>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452"/>
       <c r="B452"/>
       <c r="C452"/>
       <c r="D452"/>
       <c r="E452"/>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453"/>
       <c r="B453"/>
       <c r="C453"/>
       <c r="D453"/>
       <c r="E453"/>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454"/>
       <c r="B454"/>
       <c r="C454"/>
       <c r="D454"/>
       <c r="E454"/>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455"/>
       <c r="B455"/>
       <c r="C455"/>
       <c r="D455"/>
       <c r="E455"/>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456"/>
       <c r="B456"/>
       <c r="C456"/>
       <c r="D456"/>
       <c r="E456"/>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457"/>
       <c r="B457"/>
       <c r="C457"/>
       <c r="D457"/>
       <c r="E457"/>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458"/>
       <c r="B458"/>
       <c r="C458"/>
       <c r="D458"/>
       <c r="E458"/>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459"/>
       <c r="B459"/>
       <c r="C459"/>
       <c r="D459"/>
       <c r="E459"/>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A460"/>
       <c r="B460"/>
       <c r="C460"/>
       <c r="D460"/>
       <c r="E460"/>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461"/>
       <c r="B461"/>
       <c r="C461"/>
       <c r="D461"/>
       <c r="E461"/>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462"/>
       <c r="B462"/>
       <c r="C462"/>
       <c r="D462"/>
       <c r="E462"/>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463"/>
       <c r="B463"/>
       <c r="C463"/>
       <c r="D463"/>
       <c r="E463"/>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464"/>
       <c r="B464"/>
       <c r="C464"/>
       <c r="D464"/>
       <c r="E464"/>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A465"/>
       <c r="B465"/>
       <c r="C465"/>
       <c r="D465"/>
       <c r="E465"/>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A466"/>
       <c r="B466"/>
       <c r="C466"/>
       <c r="D466"/>
       <c r="E466"/>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A467"/>
       <c r="B467"/>
       <c r="C467"/>
       <c r="D467"/>
       <c r="E467"/>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468"/>
       <c r="B468"/>
       <c r="C468"/>
       <c r="D468"/>
       <c r="E468"/>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469"/>
       <c r="B469"/>
       <c r="C469"/>
       <c r="D469"/>
       <c r="E469"/>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470"/>
       <c r="B470"/>
       <c r="C470"/>
       <c r="D470"/>
       <c r="E470"/>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471"/>
       <c r="B471"/>
       <c r="C471"/>
       <c r="D471"/>
       <c r="E471"/>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472"/>
       <c r="B472"/>
       <c r="C472"/>
       <c r="D472"/>
       <c r="E472"/>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473"/>
       <c r="B473"/>
       <c r="C473"/>
       <c r="D473"/>
       <c r="E473"/>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474"/>
       <c r="B474"/>
       <c r="C474"/>
       <c r="D474"/>
       <c r="E474"/>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A475"/>
       <c r="B475"/>
       <c r="C475"/>
       <c r="D475"/>
       <c r="E475"/>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476"/>
       <c r="B476"/>
       <c r="C476"/>
       <c r="D476"/>
       <c r="E476"/>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477"/>
       <c r="B477"/>
       <c r="C477"/>
       <c r="D477"/>
       <c r="E477"/>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A478"/>
       <c r="B478"/>
       <c r="C478"/>
       <c r="D478"/>
       <c r="E478"/>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A479"/>
       <c r="B479"/>
       <c r="C479"/>
       <c r="D479"/>
       <c r="E479"/>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A480"/>
       <c r="B480"/>
       <c r="C480"/>
       <c r="D480"/>
       <c r="E480"/>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A481"/>
       <c r="B481"/>
       <c r="C481"/>
       <c r="D481"/>
       <c r="E481"/>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A482"/>
       <c r="B482"/>
       <c r="C482"/>
@@ -7793,7 +7810,7 @@
       <c r="E482"/>
       <c r="F482" s="1"/>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A483"/>
       <c r="B483"/>
       <c r="C483"/>
@@ -7804,7 +7821,7 @@
       <c r="H483" s="1"/>
       <c r="I483" s="1"/>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A484"/>
       <c r="B484"/>
       <c r="C484"/>
@@ -7815,7 +7832,7 @@
       <c r="H484" s="1"/>
       <c r="I484" s="1"/>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A485"/>
       <c r="B485"/>
       <c r="C485"/>
@@ -7826,7 +7843,7 @@
       <c r="H485" s="1"/>
       <c r="I485" s="1"/>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A486"/>
       <c r="B486"/>
       <c r="C486"/>
@@ -7837,7 +7854,7 @@
       <c r="H486" s="1"/>
       <c r="I486" s="1"/>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A487"/>
       <c r="B487"/>
       <c r="C487"/>
@@ -7848,7 +7865,7 @@
       <c r="H487" s="1"/>
       <c r="I487" s="1"/>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A488"/>
       <c r="B488"/>
       <c r="C488"/>
@@ -7859,7 +7876,7 @@
       <c r="H488" s="1"/>
       <c r="I488" s="1"/>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A489"/>
       <c r="B489"/>
       <c r="C489"/>
@@ -7870,7 +7887,7 @@
       <c r="H489" s="1"/>
       <c r="I489" s="1"/>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A490"/>
       <c r="B490"/>
       <c r="C490"/>
@@ -7881,7 +7898,7 @@
       <c r="H490" s="1"/>
       <c r="I490" s="1"/>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A491"/>
       <c r="B491"/>
       <c r="C491"/>
@@ -7890,7 +7907,7 @@
       <c r="F491" s="1"/>
       <c r="G491" s="1"/>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A492"/>
       <c r="B492"/>
       <c r="C492"/>
@@ -7899,7 +7916,7 @@
       <c r="F492" s="1"/>
       <c r="G492" s="1"/>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A493"/>
       <c r="B493"/>
       <c r="C493"/>
@@ -7908,7 +7925,7 @@
       <c r="F493" s="1"/>
       <c r="G493" s="1"/>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A494"/>
       <c r="B494"/>
       <c r="C494"/>
@@ -7917,7 +7934,7 @@
       <c r="F494" s="1"/>
       <c r="G494" s="1"/>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A495"/>
       <c r="B495"/>
       <c r="C495"/>
@@ -7925,14 +7942,14 @@
       <c r="E495"/>
       <c r="G495" s="1"/>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A496"/>
       <c r="B496"/>
       <c r="C496"/>
       <c r="D496"/>
       <c r="E496"/>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A497"/>
       <c r="B497"/>
       <c r="C497"/>
@@ -7940,7 +7957,7 @@
       <c r="E497"/>
       <c r="F497" s="1"/>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A498"/>
       <c r="B498"/>
       <c r="C498"/>
@@ -7948,7 +7965,7 @@
       <c r="E498"/>
       <c r="F498" s="1"/>
     </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A499"/>
       <c r="B499"/>
       <c r="C499"/>
@@ -7956,324 +7973,324 @@
       <c r="E499"/>
       <c r="F499" s="1"/>
     </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A500"/>
       <c r="B500"/>
       <c r="C500"/>
       <c r="D500"/>
       <c r="E500"/>
     </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A501"/>
       <c r="B501"/>
       <c r="C501"/>
       <c r="D501"/>
       <c r="E501"/>
     </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A502"/>
       <c r="B502"/>
       <c r="C502"/>
       <c r="D502"/>
       <c r="E502"/>
     </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A503"/>
       <c r="B503"/>
       <c r="C503"/>
       <c r="D503"/>
       <c r="E503"/>
     </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A504"/>
       <c r="B504"/>
       <c r="C504"/>
       <c r="D504"/>
       <c r="E504"/>
     </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A505"/>
       <c r="B505"/>
       <c r="C505"/>
       <c r="D505"/>
       <c r="E505"/>
     </row>
-    <row r="506" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A506"/>
       <c r="B506"/>
       <c r="C506"/>
       <c r="D506"/>
       <c r="E506"/>
     </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A507"/>
       <c r="B507"/>
       <c r="C507"/>
       <c r="D507"/>
       <c r="E507"/>
     </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A508"/>
       <c r="B508"/>
       <c r="C508"/>
       <c r="D508"/>
       <c r="E508"/>
     </row>
-    <row r="509" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A509"/>
       <c r="B509"/>
       <c r="C509"/>
       <c r="D509"/>
       <c r="E509"/>
     </row>
-    <row r="510" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A510"/>
       <c r="B510"/>
       <c r="C510"/>
       <c r="D510"/>
       <c r="E510"/>
     </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A511"/>
       <c r="B511"/>
       <c r="C511"/>
       <c r="D511"/>
       <c r="E511"/>
     </row>
-    <row r="512" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A512"/>
       <c r="B512"/>
       <c r="C512"/>
       <c r="D512"/>
       <c r="E512"/>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A513"/>
       <c r="B513"/>
       <c r="C513"/>
       <c r="D513"/>
       <c r="E513"/>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514"/>
       <c r="B514"/>
       <c r="C514"/>
       <c r="D514"/>
       <c r="E514"/>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A515"/>
       <c r="B515"/>
       <c r="C515"/>
       <c r="D515"/>
       <c r="E515"/>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A516"/>
       <c r="B516"/>
       <c r="C516"/>
       <c r="D516"/>
       <c r="E516"/>
     </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A517"/>
       <c r="B517"/>
       <c r="C517"/>
       <c r="D517"/>
       <c r="E517"/>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518"/>
       <c r="B518"/>
       <c r="C518"/>
       <c r="D518"/>
       <c r="E518"/>
     </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519"/>
       <c r="B519"/>
       <c r="C519"/>
       <c r="D519"/>
       <c r="E519"/>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520"/>
       <c r="B520"/>
       <c r="C520"/>
       <c r="D520"/>
       <c r="E520"/>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A521"/>
       <c r="B521"/>
       <c r="C521"/>
       <c r="D521"/>
       <c r="E521"/>
     </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A522"/>
       <c r="B522"/>
       <c r="C522"/>
       <c r="D522"/>
       <c r="E522"/>
     </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523"/>
       <c r="B523"/>
       <c r="C523"/>
       <c r="D523"/>
       <c r="E523"/>
     </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A524"/>
       <c r="B524"/>
       <c r="C524"/>
       <c r="D524"/>
       <c r="E524"/>
     </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525"/>
       <c r="B525"/>
       <c r="C525"/>
       <c r="D525"/>
       <c r="E525"/>
     </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A526"/>
     </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A527"/>
     </row>
-    <row r="528" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A528"/>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529"/>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530"/>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531"/>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532"/>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533"/>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534"/>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535"/>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536"/>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537"/>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538"/>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539"/>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540"/>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541"/>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542"/>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543"/>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544"/>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545"/>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546"/>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547"/>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548"/>
     </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549"/>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550"/>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551"/>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552"/>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553"/>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554"/>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555"/>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556"/>
     </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A576" s="16"/>
     </row>
-    <row r="580" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="580" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F580"/>
     </row>
-    <row r="581" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="581" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F581"/>
     </row>
-    <row r="582" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="582" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F582"/>
     </row>
-    <row r="583" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="583" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F583"/>
     </row>
-    <row r="584" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="584" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F584"/>
     </row>
-    <row r="585" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="585" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F585"/>
     </row>
-    <row r="586" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="586" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F586"/>
     </row>
-    <row r="587" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="587" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F587"/>
     </row>
-    <row r="588" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="588" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F588"/>
     </row>
-    <row r="589" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="589" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F589"/>
     </row>
-    <row r="590" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="590" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F590"/>
     </row>
-    <row r="591" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="591" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F591"/>
     </row>
-    <row r="592" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="592" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F592"/>
     </row>
-    <row r="593" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="593" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F593"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asset List update en Trello sprint 4 start
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List FPS.xlsx
+++ b/Algemeen/Asset List FPS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1115,32 +1115,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178:A180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="33" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1196,7 +1196,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1223,7 +1223,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="Q5"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1322,7 +1322,7 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="Q7"/>
       <c r="R7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="Q8"/>
       <c r="R8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1417,7 +1417,7 @@
       <c r="Q9"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1562,7 +1562,7 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1676,7 +1676,7 @@
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1704,7 +1704,7 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1786,7 +1786,7 @@
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1834,7 +1834,7 @@
       <c r="Q24"/>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1858,7 +1858,7 @@
       <c r="Q25"/>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="Q26"/>
       <c r="R26"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="Q28"/>
       <c r="R28"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1954,7 +1954,7 @@
       <c r="Q29"/>
       <c r="R29"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="Q30"/>
       <c r="R30"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2003,7 +2003,7 @@
       <c r="Q31"/>
       <c r="R31"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2029,7 +2029,7 @@
       <c r="Q32"/>
       <c r="R32"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
         <v>57</v>
       </c>
@@ -2055,7 +2055,7 @@
       <c r="Q33"/>
       <c r="R33"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>57</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="Q34"/>
       <c r="R34"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
         <v>57</v>
       </c>
@@ -2107,7 +2107,7 @@
       <c r="Q35"/>
       <c r="R35"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
         <v>57</v>
       </c>
@@ -2133,7 +2133,7 @@
       <c r="Q36"/>
       <c r="R36"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>57</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="Q37"/>
       <c r="R37"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>57</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="I38" s="16"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="I39" s="16"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -2210,7 +2210,7 @@
       <c r="I40" s="2"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>59</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>59</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>59</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
         <v>59</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>59</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
         <v>55</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
         <v>55</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="19" t="s">
         <v>55</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="19" t="s">
         <v>55</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="19" t="s">
         <v>55</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
         <v>55</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="19" t="s">
         <v>56</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="19" t="s">
         <v>56</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="19" t="s">
         <v>56</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="19" t="s">
         <v>56</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="19" t="s">
         <v>56</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="19" t="s">
         <v>56</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>56</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>60</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="19" t="s">
         <v>60</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="19" t="s">
         <v>60</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="19" t="s">
         <v>60</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>60</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
         <v>60</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -2705,8 +2705,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B74" s="7" t="s">
@@ -2720,8 +2720,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B75" s="15" t="s">
@@ -2735,8 +2735,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B76" s="8" t="s">
@@ -2750,8 +2750,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B77" s="9" t="s">
@@ -2765,8 +2765,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B78" s="10" t="s">
@@ -2780,7 +2780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>63</v>
       </c>
@@ -2795,8 +2795,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B80" s="13" t="s">
@@ -2810,7 +2810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>64</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>61</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="19" t="s">
         <v>61</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="19" t="s">
         <v>61</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="19" t="s">
         <v>61</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="19" t="s">
         <v>61</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
         <v>61</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>61</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>61</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="19" t="s">
         <v>62</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>65</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>123</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>123</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>123</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>123</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>123</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>123</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="19" t="s">
         <v>89</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="19" t="s">
         <v>89</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="19" t="s">
         <v>89</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="19" t="s">
         <v>119</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="19" t="s">
         <v>119</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="19" t="s">
         <v>119</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="19" t="s">
         <v>131</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="19" t="s">
         <v>131</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="19" t="s">
         <v>131</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>122</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>115</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -3290,8 +3290,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="19" t="s">
         <v>96</v>
       </c>
       <c r="B113" s="7" t="s">
@@ -3305,8 +3305,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="19" t="s">
         <v>96</v>
       </c>
       <c r="B114" s="15" t="s">
@@ -3320,8 +3320,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="19" t="s">
         <v>96</v>
       </c>
       <c r="B115" s="8" t="s">
@@ -3335,7 +3335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="19" t="s">
         <v>127</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>127</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="19" t="s">
         <v>127</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>121</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>67</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>67</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>67</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>86</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>86</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>86</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>118</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>118</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>118</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="19" t="s">
         <v>74</v>
       </c>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="F131"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="19" t="s">
         <v>74</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="19" t="s">
         <v>74</v>
       </c>
@@ -3607,7 +3607,7 @@
       </c>
       <c r="G133" s="14"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="19" t="s">
         <v>74</v>
       </c>
@@ -3624,7 +3624,7 @@
       <c r="F134"/>
       <c r="G134" s="14"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>74</v>
       </c>
@@ -3641,7 +3641,7 @@
       <c r="F135"/>
       <c r="G135" s="14"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>74</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="G136" s="14"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>110</v>
       </c>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="G137" s="14"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>110</v>
       </c>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="G138" s="14"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>110</v>
       </c>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="G139" s="14"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>113</v>
       </c>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="G140" s="14"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>113</v>
       </c>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="G141" s="14"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>113</v>
       </c>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="G142" s="14"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="19" t="s">
         <v>102</v>
       </c>
@@ -3769,7 +3769,7 @@
       </c>
       <c r="G143" s="14"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="19" t="s">
         <v>102</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="G144" s="14"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="19" t="s">
         <v>102</v>
       </c>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="G145" s="14"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>103</v>
       </c>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="G146" s="14"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>103</v>
       </c>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="G147" s="14"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>103</v>
       </c>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="G148" s="14"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>103</v>
       </c>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="G149" s="14"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>103</v>
       </c>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="G150" s="14"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>71</v>
       </c>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="G151" s="14"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>71</v>
       </c>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="G152" s="14"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>71</v>
       </c>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="G153" s="14"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>70</v>
       </c>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="G154" s="14"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>70</v>
       </c>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="G155" s="14"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>70</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>92</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>92</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>92</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>112</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>112</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>112</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="19" t="s">
         <v>130</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="19" t="s">
         <v>130</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="19" t="s">
         <v>130</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>78</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>78</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>78</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="19" t="s">
         <v>93</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="19" t="s">
         <v>93</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="19" t="s">
         <v>93</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="19" t="s">
         <v>94</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="19" t="s">
         <v>94</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="19" t="s">
         <v>94</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="19" t="s">
         <v>124</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="19" t="s">
         <v>124</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="19" t="s">
         <v>124</v>
       </c>
@@ -4291,8 +4291,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" s="19" t="s">
         <v>106</v>
       </c>
       <c r="B178" s="7" t="s">
@@ -4306,8 +4306,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" s="19" t="s">
         <v>106</v>
       </c>
       <c r="B179" s="15" t="s">
@@ -4321,8 +4321,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" s="19" t="s">
         <v>106</v>
       </c>
       <c r="B180" s="8" t="s">
@@ -4336,7 +4336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="19" t="s">
         <v>116</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="19" t="s">
         <v>116</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="19" t="s">
         <v>116</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="19" t="s">
         <v>117</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="19" t="s">
         <v>117</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="19" t="s">
         <v>117</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>126</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>126</v>
       </c>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="F188" s="2"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>126</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="19" t="s">
         <v>72</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="19" t="s">
         <v>72</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="19" t="s">
         <v>72</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>91</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>91</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>91</v>
       </c>
@@ -4562,8 +4562,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="19" t="s">
         <v>109</v>
       </c>
       <c r="B196" s="7" t="s">
@@ -4577,8 +4577,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="19" t="s">
         <v>109</v>
       </c>
       <c r="B197" s="15" t="s">
@@ -4592,8 +4592,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="19" t="s">
         <v>109</v>
       </c>
       <c r="B198" s="8" t="s">
@@ -4607,7 +4607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>95</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>95</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>95</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="19" t="s">
         <v>203</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="19" t="s">
         <v>203</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="19" t="s">
         <v>203</v>
       </c>
@@ -4697,8 +4697,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="19" t="s">
         <v>107</v>
       </c>
       <c r="B205" s="7" t="s">
@@ -4712,8 +4712,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="19" t="s">
         <v>107</v>
       </c>
       <c r="B206" s="15" t="s">
@@ -4727,8 +4727,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="19" t="s">
         <v>107</v>
       </c>
       <c r="B207" s="8" t="s">
@@ -4742,7 +4742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>82</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>82</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>82</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="19" t="s">
         <v>77</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="19" t="s">
         <v>77</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="19" t="s">
         <v>77</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>97</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>97</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>97</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>114</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>114</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>114</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>80</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>80</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>80</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>129</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>129</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>129</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>75</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>75</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>75</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="19" t="s">
         <v>76</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="19" t="s">
         <v>76</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="19" t="s">
         <v>76</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>79</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>79</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>79</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>99</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>99</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>99</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>83</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>83</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>83</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>84</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>84</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>84</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>73</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>73</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>73</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="19" t="s">
         <v>81</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="19" t="s">
         <v>81</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="19" t="s">
         <v>81</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="19" t="s">
         <v>81</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>81</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>81</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>128</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>128</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>128</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>68</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>68</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>68</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>68</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>68</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>68</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>105</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>105</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>105</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>104</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>104</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>104</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>69</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>69</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>69</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>111</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>111</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>111</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>88</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>88</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>88</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="19" t="s">
         <v>101</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" s="19" t="s">
         <v>101</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" s="19" t="s">
         <v>101</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" s="19" t="s">
         <v>125</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" s="19" t="s">
         <v>125</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" s="19" t="s">
         <v>125</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>90</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>90</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>90</v>
       </c>
@@ -5912,8 +5912,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A286" s="19" t="s">
         <v>108</v>
       </c>
       <c r="B286" s="7" t="s">
@@ -5927,8 +5927,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A287" s="19" t="s">
         <v>108</v>
       </c>
       <c r="B287" s="15" t="s">
@@ -5942,8 +5942,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A288" s="19" t="s">
         <v>108</v>
       </c>
       <c r="B288" s="8" t="s">
@@ -5957,7 +5957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="19" t="s">
         <v>66</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="19" t="s">
         <v>66</v>
       </c>
@@ -5987,7 +5987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="19" t="s">
         <v>66</v>
       </c>
@@ -6002,8 +6002,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A292" s="19" t="s">
         <v>98</v>
       </c>
       <c r="B292" s="7" t="s">
@@ -6017,8 +6017,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A293" s="19" t="s">
         <v>98</v>
       </c>
       <c r="B293" s="15" t="s">
@@ -6032,8 +6032,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A294" s="19" t="s">
         <v>98</v>
       </c>
       <c r="B294" s="8" t="s">
@@ -6047,7 +6047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>87</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>87</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>87</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>100</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>100</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>100</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>85</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>85</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>85</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>120</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>120</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>120</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>145</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>139</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>146</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>143</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>142</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>147</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>136</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>134</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>137</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>138</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>141</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>132</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>140</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>144</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>197</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>186</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>187</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>188</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>191</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>181</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" s="19" t="s">
         <v>196</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>198</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" s="19" t="s">
         <v>183</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" s="6" t="s">
         <v>204</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>182</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>148</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" s="19" t="s">
         <v>179</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="19" t="s">
         <v>180</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" s="19" t="s">
         <v>178</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>194</v>
       </c>
@@ -6691,7 +6691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" s="2" t="s">
         <v>201</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" s="19" t="s">
         <v>192</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" s="2" t="s">
         <v>200</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" s="19" t="s">
         <v>193</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" s="19" t="s">
         <v>176</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" s="19" t="s">
         <v>175</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" s="2" t="s">
         <v>202</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" s="19" t="s">
         <v>177</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>190</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>184</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>189</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>195</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>185</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>169</v>
       </c>
@@ -6901,7 +6901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>156</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>160</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>154</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>155</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>162</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>152</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>158</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>157</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>161</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>166</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>167</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>153</v>
       </c>
@@ -7081,7 +7081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>165</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>163</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>168</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>164</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>159</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="6" t="s">
         <v>205</v>
       </c>
@@ -7170,639 +7170,639 @@
         <v>6</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384"/>
       <c r="B384"/>
       <c r="C384"/>
       <c r="D384"/>
       <c r="E384"/>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385"/>
       <c r="B385"/>
       <c r="C385"/>
       <c r="D385"/>
       <c r="E385"/>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386"/>
       <c r="B386"/>
       <c r="C386"/>
       <c r="D386"/>
       <c r="E386"/>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387"/>
       <c r="B387"/>
       <c r="C387"/>
       <c r="D387"/>
       <c r="E387"/>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388"/>
       <c r="B388"/>
       <c r="C388"/>
       <c r="D388"/>
       <c r="E388"/>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389"/>
       <c r="B389"/>
       <c r="C389"/>
       <c r="D389"/>
       <c r="E389"/>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390"/>
       <c r="B390"/>
       <c r="C390"/>
       <c r="D390"/>
       <c r="E390"/>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391"/>
       <c r="B391"/>
       <c r="C391"/>
       <c r="D391"/>
       <c r="E391"/>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A392"/>
       <c r="B392"/>
       <c r="C392"/>
       <c r="D392"/>
       <c r="E392"/>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A393"/>
       <c r="B393"/>
       <c r="C393"/>
       <c r="D393"/>
       <c r="E393"/>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394"/>
       <c r="B394"/>
       <c r="C394"/>
       <c r="D394"/>
       <c r="E394"/>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395"/>
       <c r="B395"/>
       <c r="C395"/>
       <c r="D395"/>
       <c r="E395"/>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396"/>
       <c r="B396"/>
       <c r="C396"/>
       <c r="D396"/>
       <c r="E396"/>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D397"/>
       <c r="E397"/>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D398"/>
       <c r="E398"/>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D399"/>
       <c r="E399"/>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D400"/>
       <c r="E400"/>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D401"/>
       <c r="E401"/>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D402"/>
       <c r="E402"/>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D403"/>
       <c r="E403"/>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D404"/>
       <c r="E404"/>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D405"/>
       <c r="E405"/>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D406"/>
       <c r="E406"/>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D407"/>
       <c r="E407"/>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D408"/>
       <c r="E408"/>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D409"/>
       <c r="E409"/>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D410"/>
       <c r="E410"/>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D411"/>
       <c r="E411"/>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D412"/>
       <c r="E412"/>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D413"/>
       <c r="E413"/>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D414"/>
       <c r="E414"/>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415"/>
       <c r="B415"/>
       <c r="C415"/>
       <c r="D415"/>
       <c r="E415"/>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A416"/>
       <c r="B416"/>
       <c r="C416"/>
       <c r="D416"/>
       <c r="E416"/>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A417"/>
       <c r="B417"/>
       <c r="C417"/>
       <c r="D417"/>
       <c r="E417"/>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418"/>
       <c r="B418"/>
       <c r="C418"/>
       <c r="D418"/>
       <c r="E418"/>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A419"/>
       <c r="B419"/>
       <c r="C419"/>
       <c r="D419"/>
       <c r="E419"/>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A420"/>
       <c r="B420"/>
       <c r="C420"/>
       <c r="D420"/>
       <c r="E420"/>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421"/>
       <c r="B421"/>
       <c r="C421"/>
       <c r="D421"/>
       <c r="E421"/>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422"/>
       <c r="B422"/>
       <c r="C422"/>
       <c r="D422"/>
       <c r="E422"/>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423"/>
       <c r="B423"/>
       <c r="C423"/>
       <c r="D423"/>
       <c r="E423"/>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424"/>
       <c r="B424"/>
       <c r="C424"/>
       <c r="D424"/>
       <c r="E424"/>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425"/>
       <c r="B425"/>
       <c r="C425"/>
       <c r="D425"/>
       <c r="E425"/>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426"/>
       <c r="B426"/>
       <c r="C426"/>
       <c r="D426"/>
       <c r="E426"/>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427"/>
       <c r="B427"/>
       <c r="C427"/>
       <c r="D427"/>
       <c r="E427"/>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428"/>
       <c r="B428"/>
       <c r="C428"/>
       <c r="D428"/>
       <c r="E428"/>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A429"/>
       <c r="B429"/>
       <c r="C429"/>
       <c r="D429"/>
       <c r="E429"/>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A430"/>
       <c r="B430"/>
       <c r="C430"/>
       <c r="D430"/>
       <c r="E430"/>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A431"/>
       <c r="B431"/>
       <c r="C431"/>
       <c r="D431"/>
       <c r="E431"/>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432"/>
       <c r="B432"/>
       <c r="C432"/>
       <c r="D432"/>
       <c r="E432"/>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433"/>
       <c r="B433"/>
       <c r="C433"/>
       <c r="D433"/>
       <c r="E433"/>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434"/>
       <c r="B434"/>
       <c r="C434"/>
       <c r="D434"/>
       <c r="E434"/>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435"/>
       <c r="B435"/>
       <c r="C435"/>
       <c r="D435"/>
       <c r="E435"/>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436"/>
       <c r="B436"/>
       <c r="C436"/>
       <c r="D436"/>
       <c r="E436"/>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437"/>
       <c r="B437"/>
       <c r="C437"/>
       <c r="D437"/>
       <c r="E437"/>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438"/>
       <c r="B438"/>
       <c r="C438"/>
       <c r="D438"/>
       <c r="E438"/>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439"/>
       <c r="B439"/>
       <c r="C439"/>
       <c r="D439"/>
       <c r="E439"/>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A440"/>
       <c r="B440"/>
       <c r="C440"/>
       <c r="D440"/>
       <c r="E440"/>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A441"/>
       <c r="B441"/>
       <c r="C441"/>
       <c r="D441"/>
       <c r="E441"/>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442"/>
       <c r="B442"/>
       <c r="C442"/>
       <c r="D442"/>
       <c r="E442"/>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A443"/>
       <c r="B443"/>
       <c r="C443"/>
       <c r="D443"/>
       <c r="E443"/>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A444"/>
       <c r="B444"/>
       <c r="C444"/>
       <c r="D444"/>
       <c r="E444"/>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A445"/>
       <c r="B445"/>
       <c r="C445"/>
       <c r="D445"/>
       <c r="E445"/>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A446"/>
       <c r="B446"/>
       <c r="C446"/>
       <c r="D446"/>
       <c r="E446"/>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A447"/>
       <c r="B447"/>
       <c r="C447"/>
       <c r="D447"/>
       <c r="E447"/>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448"/>
       <c r="B448"/>
       <c r="C448"/>
       <c r="D448"/>
       <c r="E448"/>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A449"/>
       <c r="B449"/>
       <c r="C449"/>
       <c r="D449"/>
       <c r="E449"/>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A450"/>
       <c r="B450"/>
       <c r="C450"/>
       <c r="D450"/>
       <c r="E450"/>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A451"/>
       <c r="B451"/>
       <c r="C451"/>
       <c r="D451"/>
       <c r="E451"/>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A452"/>
       <c r="B452"/>
       <c r="C452"/>
       <c r="D452"/>
       <c r="E452"/>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A453"/>
       <c r="B453"/>
       <c r="C453"/>
       <c r="D453"/>
       <c r="E453"/>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454"/>
       <c r="B454"/>
       <c r="C454"/>
       <c r="D454"/>
       <c r="E454"/>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A455"/>
       <c r="B455"/>
       <c r="C455"/>
       <c r="D455"/>
       <c r="E455"/>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A456"/>
       <c r="B456"/>
       <c r="C456"/>
       <c r="D456"/>
       <c r="E456"/>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A457"/>
       <c r="B457"/>
       <c r="C457"/>
       <c r="D457"/>
       <c r="E457"/>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A458"/>
       <c r="B458"/>
       <c r="C458"/>
       <c r="D458"/>
       <c r="E458"/>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A459"/>
       <c r="B459"/>
       <c r="C459"/>
       <c r="D459"/>
       <c r="E459"/>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A460"/>
       <c r="B460"/>
       <c r="C460"/>
       <c r="D460"/>
       <c r="E460"/>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A461"/>
       <c r="B461"/>
       <c r="C461"/>
       <c r="D461"/>
       <c r="E461"/>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A462"/>
       <c r="B462"/>
       <c r="C462"/>
       <c r="D462"/>
       <c r="E462"/>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463"/>
       <c r="B463"/>
       <c r="C463"/>
       <c r="D463"/>
       <c r="E463"/>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464"/>
       <c r="B464"/>
       <c r="C464"/>
       <c r="D464"/>
       <c r="E464"/>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465"/>
       <c r="B465"/>
       <c r="C465"/>
       <c r="D465"/>
       <c r="E465"/>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466"/>
       <c r="B466"/>
       <c r="C466"/>
       <c r="D466"/>
       <c r="E466"/>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A467"/>
       <c r="B467"/>
       <c r="C467"/>
       <c r="D467"/>
       <c r="E467"/>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468"/>
       <c r="B468"/>
       <c r="C468"/>
       <c r="D468"/>
       <c r="E468"/>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A469"/>
       <c r="B469"/>
       <c r="C469"/>
       <c r="D469"/>
       <c r="E469"/>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A470"/>
       <c r="B470"/>
       <c r="C470"/>
       <c r="D470"/>
       <c r="E470"/>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A471"/>
       <c r="B471"/>
       <c r="C471"/>
       <c r="D471"/>
       <c r="E471"/>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A472"/>
       <c r="B472"/>
       <c r="C472"/>
       <c r="D472"/>
       <c r="E472"/>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A473"/>
       <c r="B473"/>
       <c r="C473"/>
       <c r="D473"/>
       <c r="E473"/>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A474"/>
       <c r="B474"/>
       <c r="C474"/>
       <c r="D474"/>
       <c r="E474"/>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A475"/>
       <c r="B475"/>
       <c r="C475"/>
       <c r="D475"/>
       <c r="E475"/>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A476"/>
       <c r="B476"/>
       <c r="C476"/>
       <c r="D476"/>
       <c r="E476"/>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A477"/>
       <c r="B477"/>
       <c r="C477"/>
       <c r="D477"/>
       <c r="E477"/>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A478"/>
       <c r="B478"/>
       <c r="C478"/>
       <c r="D478"/>
       <c r="E478"/>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A479"/>
       <c r="B479"/>
       <c r="C479"/>
       <c r="D479"/>
       <c r="E479"/>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A480"/>
       <c r="B480"/>
       <c r="C480"/>
       <c r="D480"/>
       <c r="E480"/>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A481"/>
       <c r="B481"/>
       <c r="C481"/>
       <c r="D481"/>
       <c r="E481"/>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A482"/>
       <c r="B482"/>
       <c r="C482"/>
@@ -7810,7 +7810,7 @@
       <c r="E482"/>
       <c r="F482" s="1"/>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A483"/>
       <c r="B483"/>
       <c r="C483"/>
@@ -7821,7 +7821,7 @@
       <c r="H483" s="1"/>
       <c r="I483" s="1"/>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A484"/>
       <c r="B484"/>
       <c r="C484"/>
@@ -7832,7 +7832,7 @@
       <c r="H484" s="1"/>
       <c r="I484" s="1"/>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A485"/>
       <c r="B485"/>
       <c r="C485"/>
@@ -7843,7 +7843,7 @@
       <c r="H485" s="1"/>
       <c r="I485" s="1"/>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A486"/>
       <c r="B486"/>
       <c r="C486"/>
@@ -7854,7 +7854,7 @@
       <c r="H486" s="1"/>
       <c r="I486" s="1"/>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A487"/>
       <c r="B487"/>
       <c r="C487"/>
@@ -7865,7 +7865,7 @@
       <c r="H487" s="1"/>
       <c r="I487" s="1"/>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A488"/>
       <c r="B488"/>
       <c r="C488"/>
@@ -7876,7 +7876,7 @@
       <c r="H488" s="1"/>
       <c r="I488" s="1"/>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A489"/>
       <c r="B489"/>
       <c r="C489"/>
@@ -7887,7 +7887,7 @@
       <c r="H489" s="1"/>
       <c r="I489" s="1"/>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A490"/>
       <c r="B490"/>
       <c r="C490"/>
@@ -7898,7 +7898,7 @@
       <c r="H490" s="1"/>
       <c r="I490" s="1"/>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A491"/>
       <c r="B491"/>
       <c r="C491"/>
@@ -7907,7 +7907,7 @@
       <c r="F491" s="1"/>
       <c r="G491" s="1"/>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A492"/>
       <c r="B492"/>
       <c r="C492"/>
@@ -7916,7 +7916,7 @@
       <c r="F492" s="1"/>
       <c r="G492" s="1"/>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A493"/>
       <c r="B493"/>
       <c r="C493"/>
@@ -7925,7 +7925,7 @@
       <c r="F493" s="1"/>
       <c r="G493" s="1"/>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A494"/>
       <c r="B494"/>
       <c r="C494"/>
@@ -7934,7 +7934,7 @@
       <c r="F494" s="1"/>
       <c r="G494" s="1"/>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A495"/>
       <c r="B495"/>
       <c r="C495"/>
@@ -7942,14 +7942,14 @@
       <c r="E495"/>
       <c r="G495" s="1"/>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A496"/>
       <c r="B496"/>
       <c r="C496"/>
       <c r="D496"/>
       <c r="E496"/>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A497"/>
       <c r="B497"/>
       <c r="C497"/>
@@ -7957,7 +7957,7 @@
       <c r="E497"/>
       <c r="F497" s="1"/>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A498"/>
       <c r="B498"/>
       <c r="C498"/>
@@ -7965,7 +7965,7 @@
       <c r="E498"/>
       <c r="F498" s="1"/>
     </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A499"/>
       <c r="B499"/>
       <c r="C499"/>
@@ -7973,324 +7973,324 @@
       <c r="E499"/>
       <c r="F499" s="1"/>
     </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A500"/>
       <c r="B500"/>
       <c r="C500"/>
       <c r="D500"/>
       <c r="E500"/>
     </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A501"/>
       <c r="B501"/>
       <c r="C501"/>
       <c r="D501"/>
       <c r="E501"/>
     </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A502"/>
       <c r="B502"/>
       <c r="C502"/>
       <c r="D502"/>
       <c r="E502"/>
     </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A503"/>
       <c r="B503"/>
       <c r="C503"/>
       <c r="D503"/>
       <c r="E503"/>
     </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A504"/>
       <c r="B504"/>
       <c r="C504"/>
       <c r="D504"/>
       <c r="E504"/>
     </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A505"/>
       <c r="B505"/>
       <c r="C505"/>
       <c r="D505"/>
       <c r="E505"/>
     </row>
-    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A506"/>
       <c r="B506"/>
       <c r="C506"/>
       <c r="D506"/>
       <c r="E506"/>
     </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A507"/>
       <c r="B507"/>
       <c r="C507"/>
       <c r="D507"/>
       <c r="E507"/>
     </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A508"/>
       <c r="B508"/>
       <c r="C508"/>
       <c r="D508"/>
       <c r="E508"/>
     </row>
-    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A509"/>
       <c r="B509"/>
       <c r="C509"/>
       <c r="D509"/>
       <c r="E509"/>
     </row>
-    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A510"/>
       <c r="B510"/>
       <c r="C510"/>
       <c r="D510"/>
       <c r="E510"/>
     </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A511"/>
       <c r="B511"/>
       <c r="C511"/>
       <c r="D511"/>
       <c r="E511"/>
     </row>
-    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A512"/>
       <c r="B512"/>
       <c r="C512"/>
       <c r="D512"/>
       <c r="E512"/>
     </row>
-    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A513"/>
       <c r="B513"/>
       <c r="C513"/>
       <c r="D513"/>
       <c r="E513"/>
     </row>
-    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A514"/>
       <c r="B514"/>
       <c r="C514"/>
       <c r="D514"/>
       <c r="E514"/>
     </row>
-    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A515"/>
       <c r="B515"/>
       <c r="C515"/>
       <c r="D515"/>
       <c r="E515"/>
     </row>
-    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A516"/>
       <c r="B516"/>
       <c r="C516"/>
       <c r="D516"/>
       <c r="E516"/>
     </row>
-    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A517"/>
       <c r="B517"/>
       <c r="C517"/>
       <c r="D517"/>
       <c r="E517"/>
     </row>
-    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A518"/>
       <c r="B518"/>
       <c r="C518"/>
       <c r="D518"/>
       <c r="E518"/>
     </row>
-    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A519"/>
       <c r="B519"/>
       <c r="C519"/>
       <c r="D519"/>
       <c r="E519"/>
     </row>
-    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A520"/>
       <c r="B520"/>
       <c r="C520"/>
       <c r="D520"/>
       <c r="E520"/>
     </row>
-    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A521"/>
       <c r="B521"/>
       <c r="C521"/>
       <c r="D521"/>
       <c r="E521"/>
     </row>
-    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A522"/>
       <c r="B522"/>
       <c r="C522"/>
       <c r="D522"/>
       <c r="E522"/>
     </row>
-    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A523"/>
       <c r="B523"/>
       <c r="C523"/>
       <c r="D523"/>
       <c r="E523"/>
     </row>
-    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A524"/>
       <c r="B524"/>
       <c r="C524"/>
       <c r="D524"/>
       <c r="E524"/>
     </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A525"/>
       <c r="B525"/>
       <c r="C525"/>
       <c r="D525"/>
       <c r="E525"/>
     </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A526"/>
     </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A527"/>
     </row>
-    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A528"/>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A529"/>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A530"/>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A531"/>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A532"/>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A533"/>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A534"/>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A535"/>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A536"/>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A537"/>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A538"/>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A539"/>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A540"/>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A541"/>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A542"/>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A543"/>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A544"/>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A545"/>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A546"/>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A547"/>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A548"/>
     </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A549"/>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A550"/>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A551"/>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A552"/>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A553"/>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A554"/>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A555"/>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A556"/>
     </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A576" s="16"/>
     </row>
-    <row r="580" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="580" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F580"/>
     </row>
-    <row r="581" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="581" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F581"/>
     </row>
-    <row r="582" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="582" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F582"/>
     </row>
-    <row r="583" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="583" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F583"/>
     </row>
-    <row r="584" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="584" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F584"/>
     </row>
-    <row r="585" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="585" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F585"/>
     </row>
-    <row r="586" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="586" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F586"/>
     </row>
-    <row r="587" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="587" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F587"/>
     </row>
-    <row r="588" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="588" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F588"/>
     </row>
-    <row r="589" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="589" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F589"/>
     </row>
-    <row r="590" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="590" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F590"/>
     </row>
-    <row r="591" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="591" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F591"/>
     </row>
-    <row r="592" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="592" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F592"/>
     </row>
-    <row r="593" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="593" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F593"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LightFlicker af, Airvents bezig
</commit_message>
<xml_diff>
--- a/Algemeen/Asset List FPS.xlsx
+++ b/Algemeen/Asset List FPS.xlsx
@@ -541,9 +541,6 @@
     <t>MenuManager | OptionManager | PlayerController | GunManager | GunBaseClass | GunDelegate | DamageManager | Flashlight | EnemyManager |</t>
   </si>
   <si>
-    <t>EnemyMovement | InspectObjects | Light Flicker | (Hallucinations) | UI Manager | DoorOpenClose | AirVent | Environment Events |</t>
-  </si>
-  <si>
     <t>H_OM_01</t>
   </si>
   <si>
@@ -638,6 +635,9 @@
   </si>
   <si>
     <t>Intercom | Puzzles | MeleeCombat |</t>
+  </si>
+  <si>
+    <t>EnemyMovement | InspectObjects | Light Flicker | Hallucinations | UI Manager | DoorOpenClose | AirVent | Environment Events |</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178:A180"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B202" s="7" t="s">
         <v>13</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B203" s="15" t="s">
         <v>10</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204" s="8" t="s">
         <v>14</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B322" s="11" t="s">
         <v>15</v>
@@ -6469,7 +6469,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B323" s="11" t="s">
         <v>15</v>
@@ -6484,7 +6484,7 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B324" s="11" t="s">
         <v>15</v>
@@ -6499,7 +6499,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B325" s="11" t="s">
         <v>15</v>
@@ -6514,7 +6514,7 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B326" s="11" t="s">
         <v>15</v>
@@ -6529,7 +6529,7 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B327" s="11" t="s">
         <v>15</v>
@@ -6544,7 +6544,7 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B328" s="11" t="s">
         <v>15</v>
@@ -6559,7 +6559,7 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B329" s="11" t="s">
         <v>15</v>
@@ -6574,7 +6574,7 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B330" s="11" t="s">
         <v>15</v>
@@ -6589,7 +6589,7 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B331" s="11" t="s">
         <v>15</v>
@@ -6603,7 +6603,7 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B332" s="11" t="s">
         <v>15</v>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B334" s="11" t="s">
         <v>15</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B335" s="11" t="s">
         <v>15</v>
@@ -6663,7 +6663,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B336" s="11" t="s">
         <v>15</v>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B337" s="11" t="s">
         <v>15</v>
@@ -6693,7 +6693,7 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B338" s="11" t="s">
         <v>15</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B339" s="11" t="s">
         <v>15</v>
@@ -6723,7 +6723,7 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B340" s="11" t="s">
         <v>15</v>
@@ -6738,7 +6738,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B341" s="11" t="s">
         <v>15</v>
@@ -6753,7 +6753,7 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B342" s="11" t="s">
         <v>15</v>
@@ -6768,7 +6768,7 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B343" s="11" t="s">
         <v>15</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B344" s="11" t="s">
         <v>15</v>
@@ -6798,7 +6798,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B345" s="11" t="s">
         <v>15</v>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B346" s="11" t="s">
         <v>15</v>
@@ -6828,7 +6828,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B347" s="11" t="s">
         <v>15</v>
@@ -6843,7 +6843,7 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B348" s="11" t="s">
         <v>15</v>
@@ -6858,7 +6858,7 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B349" s="11" t="s">
         <v>15</v>
@@ -6873,7 +6873,7 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B350" s="11" t="s">
         <v>15</v>
@@ -7158,7 +7158,7 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B369" s="11" t="s">
         <v>15</v>

</xml_diff>